<commit_message>
Removed Data From Dumps
</commit_message>
<xml_diff>
--- a/Main Excel.xlsx
+++ b/Main Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daily AUM Predictions\Automated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BA64FD-DAFB-40E1-97F1-D0C55943F5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C37E718-5991-43C7-8457-027E75C479AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3930,7 +3930,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>